<commit_message>
Confirmation page is pending
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testData/TestData.xlsx
+++ b/mercury/src/test/resources/testData/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15915" windowHeight="4530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MercuryLoginData" sheetId="1" r:id="rId1"/>
     <sheet name="RegisterData" sheetId="2" r:id="rId2"/>
     <sheet name="FlightData" sheetId="3" r:id="rId3"/>
+    <sheet name="Bookaflight" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>UserName</t>
   </si>
@@ -97,6 +98,118 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>meal</t>
+  </si>
+  <si>
+    <t>cardtype</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>monthExpire</t>
+  </si>
+  <si>
+    <t>yearExpire</t>
+  </si>
+  <si>
+    <t>Nameoncard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Midnameoncard</t>
+  </si>
+  <si>
+    <t>lastnameoncard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Address1stline</t>
+  </si>
+  <si>
+    <t>Address2ndline</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> city</t>
+  </si>
+  <si>
+    <t>postalcode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deladd1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deladd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  delcity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delstate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delpostal </t>
+  </si>
+  <si>
+    <t>delcountry</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Smily</t>
+  </si>
+  <si>
+    <t>Sood</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>46788584758547885</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Smile</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>Delhi(NCR)</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>1254687</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>1234587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName
+</t>
   </si>
 </sst>
 </file>
@@ -169,13 +282,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -660,4 +779,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="7" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>